<commit_message>
Added checkboxes to enable/disable the chart lines
</commit_message>
<xml_diff>
--- a/Vertaling.xlsx
+++ b/Vertaling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Nederlands</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>All tables</t>
+  </si>
+  <si>
+    <t>Toon niet op Taakbalk</t>
+  </si>
+  <si>
+    <t>Hide from task bar</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,71 +552,79 @@
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
-      <c r="C17" t="s">
+    <row r="18" spans="2:4">
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
-      <c r="C18" t="s">
+    <row r="19" spans="2:4">
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
-      <c r="C20" t="s">
+    <row r="21" spans="2:4">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
-      <c r="C21" t="s">
+    <row r="22" spans="2:4">
+      <c r="C22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
-      <c r="C22" t="s">
+    <row r="23" spans="2:4">
+      <c r="C23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
-      <c r="C23" t="s">
+    <row r="24" spans="2:4">
+      <c r="C24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
-      <c r="C24" t="s">
+    <row r="25" spans="2:4">
+      <c r="C25" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>